<commit_message>
change the time series format
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="quarter" sheetId="1" state="visible" r:id="rId2"/>
@@ -674,16 +674,16 @@
   </sheetPr>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,17 +2746,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:EP211"/>
+  <dimension ref="A1:EP210"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="9:9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A201" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CR213" activeCellId="0" sqref="CR213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -90668,15 +90668,6 @@
       <c r="EO210" s="8"/>
       <c r="EP210" s="8"/>
     </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="10" t="n">
-        <v>41061</v>
-      </c>
-      <c r="B211" s="8" t="n">
-        <f aca="false">YEAR(A211)</f>
-        <v>2012</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>